<commit_message>
🧹 LIMPEZA: Reorganização de arquivos e atualização de outputs
📁 MUDANÇAS ESTRUTURAIS:
- Removidos input_pdfs/tela1.pdf e tela3.pdf (movidos para inputs/pdf/)
- Atualizados outputs processados com dados mais recentes

📊 OUTPUTS ATUALIZADOS:
- outputs/atrib_limpos/ - Dados limpos atualizados
- outputs/csv/ - CSVs com processamento melhorado
- outputs/doc/ - Documentação normalizada atualizada
- outputs/excel/ - Planilhas com dados refinados

⚙️ CÓDIGO:
- src/app.py - Atualizações para nova arquitetura

✨ Preparação para TODO #6 com workspace limpo e organizado
</commit_message>
<xml_diff>
--- a/outputs/excel/tela1_params.xlsx
+++ b/outputs/excel/tela1_params.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10921"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/accol/Library/Mobile Documents/com~apple~CloudDocs/UNIVERSIDADES/UFF/PROJETOS/PETROBRAS/PETRO_ProtecAI/protecai_testes/outputs/excel/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB56807F-6E97-D44C-A7C4-41C8B8792E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="30080" windowHeight="19440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="micom" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -2413,8 +2407,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2477,21 +2471,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2529,7 +2515,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -2563,7 +2549,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -2598,10 +2583,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2774,19 +2758,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C339"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A158" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.83203125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2797,7 +2776,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2808,7 +2787,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2819,7 +2798,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2830,7 +2809,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2841,7 +2820,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2852,7 +2831,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -2863,7 +2842,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -2874,7 +2853,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2885,7 +2864,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -2896,7 +2875,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -2907,7 +2886,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -2918,7 +2897,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -2929,7 +2908,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -2940,7 +2919,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -2951,7 +2930,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -2962,7 +2941,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -2973,7 +2952,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -2984,7 +2963,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -2995,7 +2974,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -3006,7 +2985,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -3017,7 +2996,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -3028,7 +3007,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -3039,7 +3018,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -3050,7 +3029,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -3061,7 +3040,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -3072,7 +3051,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -3083,7 +3062,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -3094,7 +3073,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -3105,7 +3084,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -3116,7 +3095,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -3127,7 +3106,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -3138,7 +3117,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -3149,7 +3128,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -3160,7 +3139,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -3171,7 +3150,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -3182,7 +3161,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -3193,7 +3172,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -3204,7 +3183,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
         <v>40</v>
       </c>
@@ -3215,7 +3194,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -3226,7 +3205,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -3237,7 +3216,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3">
       <c r="A42" t="s">
         <v>43</v>
       </c>
@@ -3248,7 +3227,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
         <v>44</v>
       </c>
@@ -3259,7 +3238,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -3270,7 +3249,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3">
       <c r="A45" t="s">
         <v>46</v>
       </c>
@@ -3281,7 +3260,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3">
       <c r="A46" t="s">
         <v>47</v>
       </c>
@@ -3292,7 +3271,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3">
       <c r="A47" t="s">
         <v>48</v>
       </c>
@@ -3303,7 +3282,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3">
       <c r="A48" t="s">
         <v>49</v>
       </c>
@@ -3314,7 +3293,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3">
       <c r="A49" t="s">
         <v>50</v>
       </c>
@@ -3325,7 +3304,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3">
       <c r="A50" t="s">
         <v>51</v>
       </c>
@@ -3336,7 +3315,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3">
       <c r="A51" t="s">
         <v>52</v>
       </c>
@@ -3347,7 +3326,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3">
       <c r="A52" t="s">
         <v>53</v>
       </c>
@@ -3358,7 +3337,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3">
       <c r="A53" t="s">
         <v>54</v>
       </c>
@@ -3369,7 +3348,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3">
       <c r="A54" t="s">
         <v>55</v>
       </c>
@@ -3380,7 +3359,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3">
       <c r="A55" t="s">
         <v>56</v>
       </c>
@@ -3391,7 +3370,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3">
       <c r="A56" t="s">
         <v>57</v>
       </c>
@@ -3402,7 +3381,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3">
       <c r="A57" t="s">
         <v>58</v>
       </c>
@@ -3413,7 +3392,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3">
       <c r="A58" t="s">
         <v>59</v>
       </c>
@@ -3424,7 +3403,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3">
       <c r="A59" t="s">
         <v>60</v>
       </c>
@@ -3435,7 +3414,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3">
       <c r="A60" t="s">
         <v>61</v>
       </c>
@@ -3446,7 +3425,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3">
       <c r="A61" t="s">
         <v>62</v>
       </c>
@@ -3457,7 +3436,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3">
       <c r="A62" t="s">
         <v>63</v>
       </c>
@@ -3468,7 +3447,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3">
       <c r="A63" t="s">
         <v>64</v>
       </c>
@@ -3479,7 +3458,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3">
       <c r="A64" t="s">
         <v>65</v>
       </c>
@@ -3490,7 +3469,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3">
       <c r="A65" t="s">
         <v>66</v>
       </c>
@@ -3501,7 +3480,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3">
       <c r="A66" t="s">
         <v>67</v>
       </c>
@@ -3512,7 +3491,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3">
       <c r="A67" t="s">
         <v>68</v>
       </c>
@@ -3523,7 +3502,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3">
       <c r="A68" t="s">
         <v>69</v>
       </c>
@@ -3534,7 +3513,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3">
       <c r="A69" t="s">
         <v>70</v>
       </c>
@@ -3545,7 +3524,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3">
       <c r="A70" t="s">
         <v>71</v>
       </c>
@@ -3556,7 +3535,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3">
       <c r="A71" t="s">
         <v>72</v>
       </c>
@@ -3567,7 +3546,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3">
       <c r="A72" t="s">
         <v>73</v>
       </c>
@@ -3578,7 +3557,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3">
       <c r="A73" t="s">
         <v>74</v>
       </c>
@@ -3589,7 +3568,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3">
       <c r="A74" t="s">
         <v>75</v>
       </c>
@@ -3600,7 +3579,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3">
       <c r="A75" t="s">
         <v>76</v>
       </c>
@@ -3611,7 +3590,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3">
       <c r="A76" t="s">
         <v>77</v>
       </c>
@@ -3622,7 +3601,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3">
       <c r="A77" t="s">
         <v>78</v>
       </c>
@@ -3633,7 +3612,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3">
       <c r="A78" t="s">
         <v>79</v>
       </c>
@@ -3644,7 +3623,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3">
       <c r="A79" t="s">
         <v>80</v>
       </c>
@@ -3655,7 +3634,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3">
       <c r="A80" t="s">
         <v>81</v>
       </c>
@@ -3666,7 +3645,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3">
       <c r="A81" t="s">
         <v>82</v>
       </c>
@@ -3677,7 +3656,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3">
       <c r="A82" t="s">
         <v>83</v>
       </c>
@@ -3688,7 +3667,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3">
       <c r="A83" t="s">
         <v>84</v>
       </c>
@@ -3699,7 +3678,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3">
       <c r="A84" t="s">
         <v>85</v>
       </c>
@@ -3710,7 +3689,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3">
       <c r="A85" t="s">
         <v>86</v>
       </c>
@@ -3721,7 +3700,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3">
       <c r="A86" t="s">
         <v>87</v>
       </c>
@@ -3732,7 +3711,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3">
       <c r="A87" t="s">
         <v>88</v>
       </c>
@@ -3743,7 +3722,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3">
       <c r="A88" t="s">
         <v>89</v>
       </c>
@@ -3754,7 +3733,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3">
       <c r="A89" t="s">
         <v>90</v>
       </c>
@@ -3765,7 +3744,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3">
       <c r="A90" t="s">
         <v>91</v>
       </c>
@@ -3776,7 +3755,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3">
       <c r="A91" t="s">
         <v>92</v>
       </c>
@@ -3787,7 +3766,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3">
       <c r="A92" t="s">
         <v>93</v>
       </c>
@@ -3798,7 +3777,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3">
       <c r="A93" t="s">
         <v>94</v>
       </c>
@@ -3809,7 +3788,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3">
       <c r="A94" t="s">
         <v>95</v>
       </c>
@@ -3820,7 +3799,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3">
       <c r="A95" t="s">
         <v>96</v>
       </c>
@@ -3831,7 +3810,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3">
       <c r="A96" t="s">
         <v>97</v>
       </c>
@@ -3842,7 +3821,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3">
       <c r="A97" t="s">
         <v>98</v>
       </c>
@@ -3853,7 +3832,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3">
       <c r="A98" t="s">
         <v>99</v>
       </c>
@@ -3864,7 +3843,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3">
       <c r="A99" t="s">
         <v>100</v>
       </c>
@@ -3875,7 +3854,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3">
       <c r="A100" t="s">
         <v>101</v>
       </c>
@@ -3886,7 +3865,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3">
       <c r="A101" t="s">
         <v>102</v>
       </c>
@@ -3897,7 +3876,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3">
       <c r="A102" t="s">
         <v>103</v>
       </c>
@@ -3908,7 +3887,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3">
       <c r="A103" t="s">
         <v>104</v>
       </c>
@@ -3919,7 +3898,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3">
       <c r="A104" t="s">
         <v>105</v>
       </c>
@@ -3930,7 +3909,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3">
       <c r="A105" t="s">
         <v>106</v>
       </c>
@@ -3941,7 +3920,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3">
       <c r="A106" t="s">
         <v>107</v>
       </c>
@@ -3952,7 +3931,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3">
       <c r="A107" t="s">
         <v>108</v>
       </c>
@@ -3963,7 +3942,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3">
       <c r="A108" t="s">
         <v>109</v>
       </c>
@@ -3974,7 +3953,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3">
       <c r="A109" t="s">
         <v>110</v>
       </c>
@@ -3985,7 +3964,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3">
       <c r="A110" t="s">
         <v>111</v>
       </c>
@@ -3996,7 +3975,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3">
       <c r="A111" t="s">
         <v>112</v>
       </c>
@@ -4007,7 +3986,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3">
       <c r="A112" t="s">
         <v>113</v>
       </c>
@@ -4018,7 +3997,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:3">
       <c r="A113" t="s">
         <v>114</v>
       </c>
@@ -4029,7 +4008,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:3">
       <c r="A114" t="s">
         <v>115</v>
       </c>
@@ -4040,7 +4019,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:3">
       <c r="A115" t="s">
         <v>116</v>
       </c>
@@ -4051,7 +4030,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:3">
       <c r="A116" t="s">
         <v>117</v>
       </c>
@@ -4062,7 +4041,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:3">
       <c r="A117" t="s">
         <v>118</v>
       </c>
@@ -4073,7 +4052,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:3">
       <c r="A118" t="s">
         <v>119</v>
       </c>
@@ -4084,7 +4063,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:3">
       <c r="A119" t="s">
         <v>120</v>
       </c>
@@ -4095,7 +4074,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:3">
       <c r="A120" t="s">
         <v>121</v>
       </c>
@@ -4106,7 +4085,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:3">
       <c r="A121" t="s">
         <v>122</v>
       </c>
@@ -4117,7 +4096,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:3">
       <c r="A122" t="s">
         <v>123</v>
       </c>
@@ -4128,7 +4107,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:3">
       <c r="A123" t="s">
         <v>124</v>
       </c>
@@ -4139,7 +4118,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:3">
       <c r="A124" t="s">
         <v>125</v>
       </c>
@@ -4150,7 +4129,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:3">
       <c r="A125" t="s">
         <v>126</v>
       </c>
@@ -4161,7 +4140,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:3">
       <c r="A126" t="s">
         <v>127</v>
       </c>
@@ -4172,7 +4151,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:3">
       <c r="A127" t="s">
         <v>128</v>
       </c>
@@ -4183,7 +4162,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:3">
       <c r="A128" t="s">
         <v>129</v>
       </c>
@@ -4194,7 +4173,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:3">
       <c r="A129" t="s">
         <v>130</v>
       </c>
@@ -4205,7 +4184,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:3">
       <c r="A130" t="s">
         <v>131</v>
       </c>
@@ -4216,7 +4195,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:3">
       <c r="A131" t="s">
         <v>132</v>
       </c>
@@ -4227,7 +4206,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:3">
       <c r="A132" t="s">
         <v>133</v>
       </c>
@@ -4238,7 +4217,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:3">
       <c r="A133" t="s">
         <v>134</v>
       </c>
@@ -4249,7 +4228,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:3">
       <c r="A134" t="s">
         <v>135</v>
       </c>
@@ -4260,7 +4239,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:3">
       <c r="A135" t="s">
         <v>136</v>
       </c>
@@ -4271,7 +4250,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:3">
       <c r="A136" t="s">
         <v>137</v>
       </c>
@@ -4282,7 +4261,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:3">
       <c r="A137" t="s">
         <v>138</v>
       </c>
@@ -4293,7 +4272,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:3">
       <c r="A138" t="s">
         <v>139</v>
       </c>
@@ -4304,7 +4283,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:3">
       <c r="A139" t="s">
         <v>140</v>
       </c>
@@ -4315,7 +4294,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:3">
       <c r="A140" t="s">
         <v>141</v>
       </c>
@@ -4326,7 +4305,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:3">
       <c r="A141" t="s">
         <v>142</v>
       </c>
@@ -4337,7 +4316,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:3">
       <c r="A142" t="s">
         <v>143</v>
       </c>
@@ -4348,7 +4327,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:3">
       <c r="A143" t="s">
         <v>144</v>
       </c>
@@ -4359,7 +4338,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:3">
       <c r="A144" t="s">
         <v>145</v>
       </c>
@@ -4370,7 +4349,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:3">
       <c r="A145" t="s">
         <v>146</v>
       </c>
@@ -4381,7 +4360,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:3">
       <c r="A146" t="s">
         <v>147</v>
       </c>
@@ -4392,7 +4371,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:3">
       <c r="A147" t="s">
         <v>148</v>
       </c>
@@ -4403,7 +4382,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:3">
       <c r="A148" t="s">
         <v>149</v>
       </c>
@@ -4414,7 +4393,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:3">
       <c r="A149" t="s">
         <v>150</v>
       </c>
@@ -4425,7 +4404,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:3">
       <c r="A150" t="s">
         <v>151</v>
       </c>
@@ -4436,7 +4415,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:3">
       <c r="A151" t="s">
         <v>152</v>
       </c>
@@ -4447,7 +4426,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:3">
       <c r="A152" t="s">
         <v>153</v>
       </c>
@@ -4458,7 +4437,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:3">
       <c r="A153" t="s">
         <v>154</v>
       </c>
@@ -4469,7 +4448,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:3">
       <c r="A154" t="s">
         <v>155</v>
       </c>
@@ -4480,7 +4459,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:3">
       <c r="A155" t="s">
         <v>156</v>
       </c>
@@ -4491,7 +4470,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:3">
       <c r="A156" t="s">
         <v>157</v>
       </c>
@@ -4502,7 +4481,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:3">
       <c r="A157" t="s">
         <v>158</v>
       </c>
@@ -4513,7 +4492,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:3">
       <c r="A158" t="s">
         <v>159</v>
       </c>
@@ -4524,7 +4503,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:3">
       <c r="A159" t="s">
         <v>160</v>
       </c>
@@ -4535,7 +4514,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:3">
       <c r="A160" t="s">
         <v>161</v>
       </c>
@@ -4546,7 +4525,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:3">
       <c r="A161" t="s">
         <v>162</v>
       </c>
@@ -4557,7 +4536,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:3">
       <c r="A162" t="s">
         <v>163</v>
       </c>
@@ -4568,7 +4547,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:3">
       <c r="A163" t="s">
         <v>164</v>
       </c>
@@ -4579,7 +4558,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:3">
       <c r="A164" t="s">
         <v>165</v>
       </c>
@@ -4590,7 +4569,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:3">
       <c r="A165" t="s">
         <v>166</v>
       </c>
@@ -4601,7 +4580,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:3">
       <c r="A166" t="s">
         <v>167</v>
       </c>
@@ -4612,7 +4591,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:3">
       <c r="A167" t="s">
         <v>168</v>
       </c>
@@ -4623,7 +4602,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:3">
       <c r="A168" t="s">
         <v>169</v>
       </c>
@@ -4634,7 +4613,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:3">
       <c r="A169" t="s">
         <v>170</v>
       </c>
@@ -4645,7 +4624,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:3">
       <c r="A170" t="s">
         <v>171</v>
       </c>
@@ -4656,7 +4635,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:3">
       <c r="A171" t="s">
         <v>172</v>
       </c>
@@ -4667,7 +4646,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:3">
       <c r="A172" t="s">
         <v>173</v>
       </c>
@@ -4678,7 +4657,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:3">
       <c r="A173" t="s">
         <v>174</v>
       </c>
@@ -4689,7 +4668,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:3">
       <c r="A174" t="s">
         <v>175</v>
       </c>
@@ -4700,7 +4679,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:3">
       <c r="A175" t="s">
         <v>176</v>
       </c>
@@ -4711,7 +4690,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:3">
       <c r="A176" t="s">
         <v>177</v>
       </c>
@@ -4722,7 +4701,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:3">
       <c r="A177" t="s">
         <v>178</v>
       </c>
@@ -4733,7 +4712,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:3">
       <c r="A178" t="s">
         <v>179</v>
       </c>
@@ -4744,7 +4723,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:3">
       <c r="A179" t="s">
         <v>180</v>
       </c>
@@ -4755,7 +4734,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:3">
       <c r="A180" t="s">
         <v>181</v>
       </c>
@@ -4766,7 +4745,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:3">
       <c r="A181" t="s">
         <v>182</v>
       </c>
@@ -4777,7 +4756,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:3">
       <c r="A182" t="s">
         <v>183</v>
       </c>
@@ -4788,7 +4767,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:3">
       <c r="A183" t="s">
         <v>184</v>
       </c>
@@ -4799,7 +4778,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:3">
       <c r="A184" t="s">
         <v>185</v>
       </c>
@@ -4810,7 +4789,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:3">
       <c r="A185" t="s">
         <v>186</v>
       </c>
@@ -4821,7 +4800,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:3">
       <c r="A186" t="s">
         <v>187</v>
       </c>
@@ -4832,7 +4811,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:3">
       <c r="A187" t="s">
         <v>188</v>
       </c>
@@ -4843,7 +4822,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:3">
       <c r="A188" t="s">
         <v>189</v>
       </c>
@@ -4854,7 +4833,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:3">
       <c r="A189" t="s">
         <v>190</v>
       </c>
@@ -4865,7 +4844,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:3">
       <c r="A190" t="s">
         <v>191</v>
       </c>
@@ -4876,7 +4855,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:3">
       <c r="A191" t="s">
         <v>192</v>
       </c>
@@ -4887,7 +4866,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:3">
       <c r="A192" t="s">
         <v>193</v>
       </c>
@@ -4898,7 +4877,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:3">
       <c r="A193" t="s">
         <v>194</v>
       </c>
@@ -4909,7 +4888,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:3">
       <c r="A194" t="s">
         <v>195</v>
       </c>
@@ -4920,7 +4899,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:3">
       <c r="A195" t="s">
         <v>196</v>
       </c>
@@ -4931,7 +4910,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:3">
       <c r="A196" t="s">
         <v>197</v>
       </c>
@@ -4942,7 +4921,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:3">
       <c r="A197" t="s">
         <v>198</v>
       </c>
@@ -4953,7 +4932,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:3">
       <c r="A198" t="s">
         <v>199</v>
       </c>
@@ -4964,7 +4943,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:3">
       <c r="A199" t="s">
         <v>200</v>
       </c>
@@ -4975,7 +4954,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:3">
       <c r="A200" t="s">
         <v>201</v>
       </c>
@@ -4986,7 +4965,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:3">
       <c r="A201" t="s">
         <v>202</v>
       </c>
@@ -4997,7 +4976,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:3">
       <c r="A202" t="s">
         <v>203</v>
       </c>
@@ -5008,7 +4987,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:3">
       <c r="A203" t="s">
         <v>204</v>
       </c>
@@ -5019,7 +4998,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:3">
       <c r="A204" t="s">
         <v>205</v>
       </c>
@@ -5030,7 +5009,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:3">
       <c r="A205" t="s">
         <v>206</v>
       </c>
@@ -5041,7 +5020,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:3">
       <c r="A206" t="s">
         <v>207</v>
       </c>
@@ -5052,7 +5031,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:3">
       <c r="A207" t="s">
         <v>208</v>
       </c>
@@ -5063,7 +5042,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:3">
       <c r="A208" t="s">
         <v>209</v>
       </c>
@@ -5074,7 +5053,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:3">
       <c r="A209" t="s">
         <v>210</v>
       </c>
@@ -5085,7 +5064,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:3">
       <c r="A210" t="s">
         <v>211</v>
       </c>
@@ -5096,7 +5075,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:3">
       <c r="A211" t="s">
         <v>212</v>
       </c>
@@ -5107,7 +5086,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:3">
       <c r="A212" t="s">
         <v>213</v>
       </c>
@@ -5118,7 +5097,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:3">
       <c r="A213" t="s">
         <v>214</v>
       </c>
@@ -5129,7 +5108,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:3">
       <c r="A214" t="s">
         <v>215</v>
       </c>
@@ -5140,7 +5119,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:3">
       <c r="A215" t="s">
         <v>216</v>
       </c>
@@ -5151,7 +5130,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:3">
       <c r="A216" t="s">
         <v>217</v>
       </c>
@@ -5162,7 +5141,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:3">
       <c r="A217" t="s">
         <v>218</v>
       </c>
@@ -5173,7 +5152,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:3">
       <c r="A218" t="s">
         <v>219</v>
       </c>
@@ -5184,7 +5163,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:3">
       <c r="A219" t="s">
         <v>220</v>
       </c>
@@ -5195,7 +5174,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:3">
       <c r="A220" t="s">
         <v>221</v>
       </c>
@@ -5206,7 +5185,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:3">
       <c r="A221" t="s">
         <v>222</v>
       </c>
@@ -5217,7 +5196,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:3">
       <c r="A222" t="s">
         <v>223</v>
       </c>
@@ -5228,7 +5207,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:3">
       <c r="A223" t="s">
         <v>224</v>
       </c>
@@ -5239,7 +5218,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:3">
       <c r="A224" t="s">
         <v>225</v>
       </c>
@@ -5250,7 +5229,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:3">
       <c r="A225" t="s">
         <v>226</v>
       </c>
@@ -5261,7 +5240,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:3">
       <c r="A226" t="s">
         <v>227</v>
       </c>
@@ -5272,7 +5251,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:3">
       <c r="A227" t="s">
         <v>228</v>
       </c>
@@ -5283,7 +5262,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:3">
       <c r="A228" t="s">
         <v>229</v>
       </c>
@@ -5294,7 +5273,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:3">
       <c r="A229" t="s">
         <v>230</v>
       </c>
@@ -5305,7 +5284,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:3">
       <c r="A230" t="s">
         <v>231</v>
       </c>
@@ -5316,7 +5295,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:3">
       <c r="A231" t="s">
         <v>232</v>
       </c>
@@ -5327,7 +5306,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:3">
       <c r="A232" t="s">
         <v>233</v>
       </c>
@@ -5338,7 +5317,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:3">
       <c r="A233" t="s">
         <v>234</v>
       </c>
@@ -5349,7 +5328,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:3">
       <c r="A234" t="s">
         <v>235</v>
       </c>
@@ -5360,7 +5339,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:3">
       <c r="A235" t="s">
         <v>236</v>
       </c>
@@ -5371,7 +5350,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:3">
       <c r="A236" t="s">
         <v>237</v>
       </c>
@@ -5382,7 +5361,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:3">
       <c r="A237" t="s">
         <v>238</v>
       </c>
@@ -5393,7 +5372,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:3">
       <c r="A238" t="s">
         <v>239</v>
       </c>
@@ -5404,7 +5383,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:3">
       <c r="A239" t="s">
         <v>240</v>
       </c>
@@ -5415,7 +5394,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:3">
       <c r="A240" t="s">
         <v>241</v>
       </c>
@@ -5426,7 +5405,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:3">
       <c r="A241" t="s">
         <v>242</v>
       </c>
@@ -5437,7 +5416,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:3">
       <c r="A242" t="s">
         <v>243</v>
       </c>
@@ -5448,7 +5427,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:3">
       <c r="A243" t="s">
         <v>244</v>
       </c>
@@ -5459,7 +5438,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:3">
       <c r="A244" t="s">
         <v>245</v>
       </c>
@@ -5470,7 +5449,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:3">
       <c r="A245" t="s">
         <v>246</v>
       </c>
@@ -5481,7 +5460,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:3">
       <c r="A246" t="s">
         <v>247</v>
       </c>
@@ -5492,7 +5471,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:3">
       <c r="A247" t="s">
         <v>248</v>
       </c>
@@ -5503,7 +5482,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:3">
       <c r="A248" t="s">
         <v>249</v>
       </c>
@@ -5511,7 +5490,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:3">
       <c r="A249" t="s">
         <v>250</v>
       </c>
@@ -5522,7 +5501,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:3">
       <c r="A250" t="s">
         <v>251</v>
       </c>
@@ -5533,7 +5512,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:3">
       <c r="A251" t="s">
         <v>252</v>
       </c>
@@ -5544,7 +5523,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:3">
       <c r="A252" t="s">
         <v>253</v>
       </c>
@@ -5555,7 +5534,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:3">
       <c r="A253" t="s">
         <v>254</v>
       </c>
@@ -5566,7 +5545,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:3">
       <c r="A254" t="s">
         <v>255</v>
       </c>
@@ -5577,7 +5556,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:3">
       <c r="A255" t="s">
         <v>256</v>
       </c>
@@ -5588,7 +5567,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:3">
       <c r="A256" t="s">
         <v>257</v>
       </c>
@@ -5599,7 +5578,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:3">
       <c r="A257" t="s">
         <v>258</v>
       </c>
@@ -5610,7 +5589,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:3">
       <c r="A258" t="s">
         <v>259</v>
       </c>
@@ -5621,7 +5600,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:3">
       <c r="A259" t="s">
         <v>260</v>
       </c>
@@ -5632,7 +5611,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:3">
       <c r="A260" t="s">
         <v>261</v>
       </c>
@@ -5643,7 +5622,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:3">
       <c r="A261" t="s">
         <v>262</v>
       </c>
@@ -5654,7 +5633,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:3">
       <c r="A262" t="s">
         <v>263</v>
       </c>
@@ -5665,7 +5644,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:3">
       <c r="A263" t="s">
         <v>264</v>
       </c>
@@ -5676,7 +5655,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:3">
       <c r="A264" t="s">
         <v>265</v>
       </c>
@@ -5687,7 +5666,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:3">
       <c r="A265" t="s">
         <v>266</v>
       </c>
@@ -5698,7 +5677,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:3">
       <c r="A266" t="s">
         <v>267</v>
       </c>
@@ -5709,7 +5688,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:3">
       <c r="A267" t="s">
         <v>268</v>
       </c>
@@ -5720,7 +5699,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:3">
       <c r="A268" t="s">
         <v>269</v>
       </c>
@@ -5731,7 +5710,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:3">
       <c r="A269" t="s">
         <v>270</v>
       </c>
@@ -5742,7 +5721,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:3">
       <c r="A270" t="s">
         <v>271</v>
       </c>
@@ -5753,7 +5732,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:3">
       <c r="A271" t="s">
         <v>272</v>
       </c>
@@ -5764,7 +5743,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:3">
       <c r="A272" t="s">
         <v>273</v>
       </c>
@@ -5772,7 +5751,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:3">
       <c r="A273" t="s">
         <v>274</v>
       </c>
@@ -5783,7 +5762,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:3">
       <c r="A274" t="s">
         <v>275</v>
       </c>
@@ -5794,7 +5773,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:3">
       <c r="A275" t="s">
         <v>276</v>
       </c>
@@ -5805,7 +5784,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:3">
       <c r="A276" t="s">
         <v>277</v>
       </c>
@@ -5816,7 +5795,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:3">
       <c r="A277" t="s">
         <v>278</v>
       </c>
@@ -5827,7 +5806,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:3">
       <c r="A278" t="s">
         <v>279</v>
       </c>
@@ -5838,7 +5817,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:3">
       <c r="A279" t="s">
         <v>280</v>
       </c>
@@ -5849,7 +5828,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:3">
       <c r="A280" t="s">
         <v>281</v>
       </c>
@@ -5860,7 +5839,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:3">
       <c r="A281" t="s">
         <v>282</v>
       </c>
@@ -5871,7 +5850,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:3">
       <c r="A282" t="s">
         <v>283</v>
       </c>
@@ -5879,7 +5858,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:3">
       <c r="A283" t="s">
         <v>284</v>
       </c>
@@ -5890,7 +5869,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:3">
       <c r="A284" t="s">
         <v>285</v>
       </c>
@@ -5901,7 +5880,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:3">
       <c r="A285" t="s">
         <v>286</v>
       </c>
@@ -5912,7 +5891,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:3">
       <c r="A286" t="s">
         <v>287</v>
       </c>
@@ -5923,7 +5902,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:3">
       <c r="A287" t="s">
         <v>288</v>
       </c>
@@ -5934,7 +5913,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:3">
       <c r="A288" t="s">
         <v>289</v>
       </c>
@@ -5945,7 +5924,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:3">
       <c r="A289" t="s">
         <v>290</v>
       </c>
@@ -5956,7 +5935,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:3">
       <c r="A290" t="s">
         <v>291</v>
       </c>
@@ -5967,7 +5946,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:3">
       <c r="A291" t="s">
         <v>292</v>
       </c>
@@ -5978,7 +5957,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:3">
       <c r="A292" t="s">
         <v>293</v>
       </c>
@@ -5989,7 +5968,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:3">
       <c r="A293" t="s">
         <v>294</v>
       </c>
@@ -6000,7 +5979,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:3">
       <c r="A294" t="s">
         <v>295</v>
       </c>
@@ -6011,7 +5990,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:3">
       <c r="A295" t="s">
         <v>296</v>
       </c>
@@ -6022,7 +6001,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:3">
       <c r="A296" t="s">
         <v>297</v>
       </c>
@@ -6033,7 +6012,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:3">
       <c r="A297" t="s">
         <v>298</v>
       </c>
@@ -6044,7 +6023,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:3">
       <c r="A298" t="s">
         <v>299</v>
       </c>
@@ -6055,7 +6034,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:3">
       <c r="A299" t="s">
         <v>300</v>
       </c>
@@ -6066,7 +6045,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:3">
       <c r="A300" t="s">
         <v>301</v>
       </c>
@@ -6077,7 +6056,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:3">
       <c r="A301" t="s">
         <v>302</v>
       </c>
@@ -6088,7 +6067,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:3">
       <c r="A302" t="s">
         <v>303</v>
       </c>
@@ -6099,7 +6078,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:3">
       <c r="A303" t="s">
         <v>304</v>
       </c>
@@ -6110,7 +6089,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:3">
       <c r="A304" t="s">
         <v>305</v>
       </c>
@@ -6121,7 +6100,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:3">
       <c r="A305" t="s">
         <v>306</v>
       </c>
@@ -6132,7 +6111,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:3">
       <c r="A306" t="s">
         <v>307</v>
       </c>
@@ -6143,7 +6122,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:3">
       <c r="A307" t="s">
         <v>308</v>
       </c>
@@ -6154,7 +6133,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:3">
       <c r="A308" t="s">
         <v>309</v>
       </c>
@@ -6165,7 +6144,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:3">
       <c r="A309" t="s">
         <v>310</v>
       </c>
@@ -6176,7 +6155,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:3">
       <c r="A310" t="s">
         <v>311</v>
       </c>
@@ -6187,7 +6166,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:3">
       <c r="A311" t="s">
         <v>312</v>
       </c>
@@ -6198,7 +6177,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:3">
       <c r="A312" t="s">
         <v>313</v>
       </c>
@@ -6209,7 +6188,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:3">
       <c r="A313" t="s">
         <v>314</v>
       </c>
@@ -6220,7 +6199,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:3">
       <c r="A314" t="s">
         <v>315</v>
       </c>
@@ -6231,7 +6210,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:3">
       <c r="A315" t="s">
         <v>316</v>
       </c>
@@ -6239,7 +6218,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:3">
       <c r="A316" t="s">
         <v>317</v>
       </c>
@@ -6250,7 +6229,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:3">
       <c r="A317" t="s">
         <v>318</v>
       </c>
@@ -6258,7 +6237,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:3">
       <c r="A318" t="s">
         <v>319</v>
       </c>
@@ -6269,7 +6248,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:3">
       <c r="A319" t="s">
         <v>320</v>
       </c>
@@ -6280,7 +6259,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:3">
       <c r="A320" t="s">
         <v>321</v>
       </c>
@@ -6291,7 +6270,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="321" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:3">
       <c r="A321" t="s">
         <v>322</v>
       </c>
@@ -6302,7 +6281,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="322" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:3">
       <c r="A322" t="s">
         <v>323</v>
       </c>
@@ -6313,7 +6292,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="323" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:3">
       <c r="A323" t="s">
         <v>324</v>
       </c>
@@ -6324,7 +6303,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="324" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:3">
       <c r="A324" t="s">
         <v>325</v>
       </c>
@@ -6335,7 +6314,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="325" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:3">
       <c r="A325" t="s">
         <v>326</v>
       </c>
@@ -6346,7 +6325,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="326" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:3">
       <c r="A326" t="s">
         <v>327</v>
       </c>
@@ -6357,7 +6336,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="327" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:3">
       <c r="A327" t="s">
         <v>328</v>
       </c>
@@ -6368,7 +6347,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="328" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:3">
       <c r="A328" t="s">
         <v>329</v>
       </c>
@@ -6379,7 +6358,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="329" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:3">
       <c r="A329" t="s">
         <v>330</v>
       </c>
@@ -6390,7 +6369,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="330" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:3">
       <c r="A330" t="s">
         <v>331</v>
       </c>
@@ -6401,7 +6380,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="331" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:3">
       <c r="A331" t="s">
         <v>332</v>
       </c>
@@ -6412,7 +6391,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="332" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:3">
       <c r="A332" t="s">
         <v>333</v>
       </c>
@@ -6423,7 +6402,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="333" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:3">
       <c r="A333" t="s">
         <v>334</v>
       </c>
@@ -6434,7 +6413,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="334" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:3">
       <c r="A334" t="s">
         <v>335</v>
       </c>
@@ -6445,7 +6424,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="335" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:3">
       <c r="A335" t="s">
         <v>336</v>
       </c>
@@ -6456,7 +6435,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="336" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:3">
       <c r="A336" t="s">
         <v>337</v>
       </c>
@@ -6467,7 +6446,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="337" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:3">
       <c r="A337" t="s">
         <v>338</v>
       </c>
@@ -6478,7 +6457,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="338" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:3">
       <c r="A338" t="s">
         <v>339</v>
       </c>
@@ -6489,7 +6468,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="339" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:3">
       <c r="A339" t="s">
         <v>340</v>
       </c>

</xml_diff>